<commit_message>
Update project versions, add support for netstandar2.0/2.1, minor changes, README.txt and CHANGELOG.md
</commit_message>
<xml_diff>
--- a/src/test/iXlsxWriter.ConsoleAppCore/Output/Sample01/Sample-01.xlsx
+++ b/src/test/iXlsxWriter.ConsoleAppCore/Output/Sample01/Sample-01.xlsx
@@ -420,18 +420,18 @@
   </cellXfs>
   <cellStyles count="35">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="aemnbnyy" xfId="1"/>
-    <cellStyle name="aemnbnyy_Alternate" xfId="2"/>
-    <cellStyle name="bysxafmy" xfId="3"/>
-    <cellStyle name="bysxafmy_Alternate" xfId="4"/>
-    <cellStyle name="jye5hv3q" xfId="5"/>
-    <cellStyle name="jye5hv3q_Alternate" xfId="6"/>
-    <cellStyle name="cakpzab1" xfId="7"/>
-    <cellStyle name="cakpzab1_Alternate" xfId="8"/>
-    <cellStyle name="qohz2kms" xfId="9"/>
-    <cellStyle name="qohz2kms_Alternate" xfId="10"/>
-    <cellStyle name="kpk5x50k" xfId="11"/>
-    <cellStyle name="kpk5x50k_Alternate" xfId="12"/>
+    <cellStyle name="1rknrrr5" xfId="1"/>
+    <cellStyle name="1rknrrr5_Alternate" xfId="2"/>
+    <cellStyle name="sjynhcei" xfId="3"/>
+    <cellStyle name="sjynhcei_Alternate" xfId="4"/>
+    <cellStyle name="vg3mc3zk" xfId="5"/>
+    <cellStyle name="vg3mc3zk_Alternate" xfId="6"/>
+    <cellStyle name="5lemomdc" xfId="7"/>
+    <cellStyle name="5lemomdc_Alternate" xfId="8"/>
+    <cellStyle name="0wrkprhg" xfId="9"/>
+    <cellStyle name="0wrkprhg_Alternate" xfId="10"/>
+    <cellStyle name="mljwhak2" xfId="11"/>
+    <cellStyle name="mljwhak2_Alternate" xfId="12"/>
     <cellStyle name="LocalHeader-1" xfId="13"/>
     <cellStyle name="LocalHeader-1_Alternate" xfId="14"/>
     <cellStyle name="LocalHeader0" xfId="15"/>
@@ -450,10 +450,10 @@
     <cellStyle name="LocalHeader6_Alternate" xfId="28"/>
     <cellStyle name="LocalHeader7" xfId="29"/>
     <cellStyle name="LocalHeader7_Alternate" xfId="30"/>
-    <cellStyle name="cvbiy1b2" xfId="31"/>
-    <cellStyle name="cvbiy1b2_Alternate" xfId="32"/>
-    <cellStyle name="bfjjgqkw" xfId="33"/>
-    <cellStyle name="bfjjgqkw_Alternate" xfId="34"/>
+    <cellStyle name="ffobxwfh" xfId="31"/>
+    <cellStyle name="ffobxwfh_Alternate" xfId="32"/>
+    <cellStyle name="shtks3xk" xfId="33"/>
+    <cellStyle name="shtks3xk_Alternate" xfId="34"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>

</xml_diff>